<commit_message>
Fix demo programs 3 and 33
</commit_message>
<xml_diff>
--- a/src/demos/zdemo_excel15_01.w3mi.data.xlsx
+++ b/src/demos/zdemo_excel15_01.w3mi.data.xlsx
@@ -419,10 +419,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="B3" s="2">
-        <v>44557</v>
+        <v>44561</v>
       </c>
       <c r="C3" s="3">
-        <v>0.7721990740740741</v>
+        <v>0.2488078703703704</v>
       </c>
     </row>
     <row r="4" spans="1:3">

</xml_diff>

<commit_message>
updated reader reference files
( affected by #935 )
</commit_message>
<xml_diff>
--- a/src/demos/zdemo_excel15_01.w3mi.data.xlsx
+++ b/src/demos/zdemo_excel15_01.w3mi.data.xlsx
@@ -248,7 +248,7 @@
         <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -386,9 +386,9 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst/>
+  <a:objectDefaults xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+  <a:extraClrSchemeLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+  <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
 </a:theme>
 </file>
 

</xml_diff>

<commit_message>
Fix demo programs 3 and 33 (#956)
* Fix demo programs 3 and 33

* updated reader reference files

( affected by #935 )

Co-authored-by: sandraros <sandra.rossi@gmail.com>
Co-authored-by: Lars Hvam <larshp@hotmail.com>
Co-authored-by: Abo <andrea@borgia.bo.it>
</commit_message>
<xml_diff>
--- a/src/demos/zdemo_excel15_01.w3mi.data.xlsx
+++ b/src/demos/zdemo_excel15_01.w3mi.data.xlsx
@@ -248,7 +248,7 @@
         <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -386,9 +386,9 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst/>
+  <a:objectDefaults xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+  <a:extraClrSchemeLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+  <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
 </a:theme>
 </file>
 
@@ -419,10 +419,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="B3" s="2">
-        <v>44557</v>
+        <v>44561</v>
       </c>
       <c r="C3" s="3">
-        <v>0.7721990740740741</v>
+        <v>0.2488078703703704</v>
       </c>
     </row>
     <row r="4" spans="1:3">

</xml_diff>